<commit_message>
to commit first changes Family
</commit_message>
<xml_diff>
--- a/BR_Family.xlsx
+++ b/BR_Family.xlsx
@@ -799,18 +799,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -819,6 +815,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -829,32 +843,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1162,7 +1162,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J47" sqref="J47"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1184,28 +1184,28 @@
       <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="62.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="33" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="18"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1218,16 +1218,16 @@
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="30" t="s">
+      <c r="J3" s="17" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
       <c r="G4" s="26"/>
       <c r="H4" s="26"/>
       <c r="I4" s="27"/>
-      <c r="J4" s="34"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
@@ -1261,7 +1261,7 @@
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="21"/>
-      <c r="J5" s="34"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
@@ -1305,7 +1305,7 @@
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
       <c r="I7" s="21"/>
-      <c r="J7" s="34"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
@@ -1349,7 +1349,7 @@
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="21"/>
-      <c r="J9" s="34"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10" ht="319" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
@@ -1466,18 +1466,18 @@
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="34"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="18"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
@@ -1495,7 +1495,7 @@
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="34"/>
+      <c r="J16" s="18"/>
     </row>
     <row r="17" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
@@ -1539,7 +1539,7 @@
       <c r="G18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="21"/>
-      <c r="J18" s="34"/>
+      <c r="J18" s="18"/>
     </row>
     <row r="19" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
@@ -1583,7 +1583,7 @@
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
       <c r="I20" s="21"/>
-      <c r="J20" s="34"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
@@ -1627,7 +1627,7 @@
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="34"/>
+      <c r="J22" s="18"/>
     </row>
     <row r="23" spans="1:10" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
@@ -1671,7 +1671,7 @@
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="21"/>
-      <c r="J24" s="34"/>
+      <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
@@ -1740,16 +1740,16 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="34"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
@@ -1767,7 +1767,7 @@
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="34"/>
+      <c r="J29" s="18"/>
     </row>
     <row r="30" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
@@ -1811,7 +1811,7 @@
       <c r="G31" s="20"/>
       <c r="H31" s="20"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="34"/>
+      <c r="J31" s="18"/>
     </row>
     <row r="32" spans="1:10" ht="116" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
@@ -1855,7 +1855,7 @@
       <c r="G33" s="20"/>
       <c r="H33" s="20"/>
       <c r="I33" s="21"/>
-      <c r="J33" s="34"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
@@ -1943,7 +1943,7 @@
       <c r="G37" s="20"/>
       <c r="H37" s="20"/>
       <c r="I37" s="21"/>
-      <c r="J37" s="34"/>
+      <c r="J37" s="18"/>
     </row>
     <row r="38" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
@@ -1987,7 +1987,7 @@
       <c r="G39" s="20"/>
       <c r="H39" s="20"/>
       <c r="I39" s="21"/>
-      <c r="J39" s="34"/>
+      <c r="J39" s="18"/>
     </row>
     <row r="40" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
@@ -2031,7 +2031,7 @@
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
       <c r="I41" s="21"/>
-      <c r="J41" s="34"/>
+      <c r="J41" s="18"/>
     </row>
     <row r="42" spans="1:10" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
@@ -2075,7 +2075,7 @@
       <c r="G43" s="20"/>
       <c r="H43" s="20"/>
       <c r="I43" s="21"/>
-      <c r="J43" s="34"/>
+      <c r="J43" s="18"/>
     </row>
     <row r="44" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
@@ -2119,7 +2119,7 @@
       <c r="G45" s="20"/>
       <c r="H45" s="20"/>
       <c r="I45" s="21"/>
-      <c r="J45" s="34"/>
+      <c r="J45" s="18"/>
     </row>
     <row r="46" spans="1:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
@@ -2163,7 +2163,7 @@
       <c r="G47" s="20"/>
       <c r="H47" s="20"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="34"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
@@ -2457,6 +2457,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C28:I28"/>
     <mergeCell ref="C47:I47"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="C45:I45"/>
@@ -2473,17 +2484,6 @@
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="C26:I26"/>
     <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>